<commit_message>
current show is ok,wait SOC
</commit_message>
<xml_diff>
--- a/ZTR引脚定义.xlsx
+++ b/ZTR引脚定义.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
@@ -439,14 +439,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OUTPUT3  控制LED（充电或者放电闪烁）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OUTPUT4    控制LED（充电或者放电闪烁）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>void Led_Init(void)</t>
   </si>
   <si>
@@ -941,13 +933,21 @@
   </si>
   <si>
     <t>Fault_CLR 错误信息清除引脚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUT3  控制LED（充电闪烁）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUT4    控制LED（运行常亮）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1205,11 +1205,16 @@
       <color rgb="FF1364AD"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1283,6 +1288,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1317,6 +1323,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1492,11 +1499,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1541,7 +1548,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>66</v>
@@ -1560,7 +1567,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>10</v>
@@ -1585,7 +1592,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>111</v>
+        <v>252</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>69</v>
@@ -1702,7 +1709,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>112</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1793,7 +1800,7 @@
         <v>46</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1817,7 +1824,7 @@
         <v>49</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1991,581 +1998,581 @@
         <v>108</v>
       </c>
       <c r="B59" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="B61" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="B62" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="27">
       <c r="A65" s="3"/>
       <c r="B65" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
+        <v>124</v>
+      </c>
+      <c r="B67" t="s">
+        <v>125</v>
+      </c>
+      <c r="C67" t="s">
         <v>126</v>
-      </c>
-      <c r="B67" t="s">
-        <v>127</v>
-      </c>
-      <c r="C67" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B69" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C69" s="23" t="s">
         <v>129</v>
-      </c>
-      <c r="B69" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="C69" s="23" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="23"/>
       <c r="B70" s="23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="23"/>
       <c r="B71" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="23"/>
       <c r="B72" s="23" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="23"/>
       <c r="B73" s="23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C73" s="23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C75" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="5"/>
       <c r="B76" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C76" s="25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="B78" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C78" s="24" t="s">
         <v>145</v>
-      </c>
-      <c r="B78" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="C78" s="24" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="24"/>
       <c r="B79" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="24"/>
       <c r="B80" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B82" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C82" s="26" t="s">
         <v>152</v>
-      </c>
-      <c r="B82" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="C82" s="26" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="26"/>
       <c r="B83" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C83" s="26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="26"/>
       <c r="B84" s="26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C84" s="26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="26"/>
       <c r="B85" s="26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C85" s="26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="26"/>
       <c r="B86" s="26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C86" s="26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B88" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="C88" s="27" t="s">
         <v>163</v>
-      </c>
-      <c r="B88" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="C88" s="27" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="27"/>
       <c r="B89" s="27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C89" s="27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="B91" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="B91" s="28" t="s">
-        <v>170</v>
-      </c>
       <c r="C91" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="28"/>
       <c r="B92" s="28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="28"/>
       <c r="B93" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C93" s="28" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="28"/>
       <c r="B94" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C94" s="28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="28"/>
       <c r="B95" s="28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C95" s="28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="28"/>
       <c r="B96" s="28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="28"/>
       <c r="B97" s="28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C97" s="28" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="28"/>
       <c r="B98" s="28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C98" s="28" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="28"/>
       <c r="B99" s="28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C99" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="28"/>
       <c r="B100" s="28" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C100" s="28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="28"/>
       <c r="B101" s="28" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C101" s="28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="28"/>
       <c r="B102" s="28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C102" s="28" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="28"/>
       <c r="B103" s="28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C103" s="28" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C105" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="4"/>
       <c r="B106" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="4"/>
       <c r="B107" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="4"/>
       <c r="B108" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="4"/>
       <c r="B109" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="4"/>
       <c r="B111" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="4"/>
       <c r="B112" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="4"/>
       <c r="B113" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="4"/>
       <c r="B114" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="27">
       <c r="A115" s="4"/>
       <c r="B115" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C115" s="30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="4"/>
       <c r="B117" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C119" s="8" t="s">
         <v>224</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="C119" s="8" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="8"/>
       <c r="B120" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C120" s="8" t="s">
         <v>227</v>
-      </c>
-      <c r="C120" s="8" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="8"/>
       <c r="B121" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C121" s="8" t="s">
         <v>228</v>
-      </c>
-      <c r="C121" s="8" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="8"/>
       <c r="B122" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="8"/>
       <c r="B123" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="8"/>
       <c r="B124" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
+        <v>235</v>
+      </c>
+      <c r="B126" t="s">
+        <v>236</v>
+      </c>
+      <c r="C126" s="8" t="s">
         <v>237</v>
-      </c>
-      <c r="B126" t="s">
-        <v>238</v>
-      </c>
-      <c r="C126" s="8" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="40.5">
       <c r="B127" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C127" s="29" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="B128" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C128" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="129" spans="2:3">
       <c r="B129" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C129" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="130" spans="2:3">
       <c r="B130" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C130" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="131" spans="2:3">
       <c r="B131" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C131" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="132" spans="2:3">
       <c r="B132" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C132" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2576,7 +2583,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2590,7 +2597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
CAN 125k add more agreement
</commit_message>
<xml_diff>
--- a/ZTR引脚定义.xlsx
+++ b/ZTR引脚定义.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
@@ -62,10 +62,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Heater Control 控制加温装置启停端口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>B0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -943,11 +939,15 @@
     <t>OUTPUT4    控制LED（运行常亮）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>故障信息指示灯（红）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1214,7 +1214,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1288,7 +1288,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1323,7 +1322,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1499,11 +1497,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1515,10 +1513,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="27">
       <c r="B1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1529,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="6" customFormat="1">
@@ -1540,7 +1538,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1548,10 +1546,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1562,18 +1560,18 @@
         <v>9</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1584,7 +1582,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1592,10 +1590,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1603,94 +1601,94 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>12</v>
+        <v>253</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="B10" s="14"/>
       <c r="C10" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:3" s="6" customFormat="1">
       <c r="A12" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1698,66 +1696,66 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1765,66 +1763,66 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1832,34 +1830,34 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1867,15 +1865,15 @@
     </row>
     <row r="43" spans="1:3" ht="27">
       <c r="B43" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>1</v>
@@ -1883,696 +1881,696 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="133.5" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="21" t="s">
         <v>97</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="3"/>
       <c r="B55" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="3"/>
       <c r="B56" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="3"/>
       <c r="B57" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B59" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" t="s">
+        <v>112</v>
+      </c>
+      <c r="C60" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="B61" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="B62" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="27">
       <c r="A65" s="3"/>
       <c r="B65" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C65" s="22" t="s">
         <v>122</v>
-      </c>
-      <c r="C65" s="22" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
+        <v>123</v>
+      </c>
+      <c r="B67" t="s">
         <v>124</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>125</v>
-      </c>
-      <c r="C67" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B69" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="B69" s="23" t="s">
+      <c r="C69" s="23" t="s">
         <v>128</v>
-      </c>
-      <c r="C69" s="23" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="23"/>
       <c r="B70" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C70" s="23" t="s">
         <v>130</v>
-      </c>
-      <c r="C70" s="23" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="23"/>
       <c r="B71" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C71" s="23" t="s">
         <v>132</v>
-      </c>
-      <c r="C71" s="23" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="23"/>
       <c r="B72" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C72" s="23" t="s">
         <v>134</v>
-      </c>
-      <c r="C72" s="23" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="23"/>
       <c r="B73" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" s="23" t="s">
         <v>136</v>
-      </c>
-      <c r="C73" s="23" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="C75" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="5"/>
       <c r="B76" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C76" s="25" t="s">
         <v>141</v>
-      </c>
-      <c r="C76" s="25" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B78" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="B78" s="24" t="s">
+      <c r="C78" s="24" t="s">
         <v>144</v>
-      </c>
-      <c r="C78" s="24" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="24"/>
       <c r="B79" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="24"/>
       <c r="B80" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C80" s="24" t="s">
         <v>147</v>
-      </c>
-      <c r="C80" s="24" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B82" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="B82" s="26" t="s">
+      <c r="C82" s="26" t="s">
         <v>151</v>
-      </c>
-      <c r="C82" s="26" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="26"/>
       <c r="B83" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C83" s="26" t="s">
         <v>153</v>
-      </c>
-      <c r="C83" s="26" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="26"/>
       <c r="B84" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C84" s="26" t="s">
         <v>155</v>
-      </c>
-      <c r="C84" s="26" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="26"/>
       <c r="B85" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="C85" s="26" t="s">
         <v>157</v>
-      </c>
-      <c r="C85" s="26" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="26"/>
       <c r="B86" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="C86" s="26" t="s">
         <v>159</v>
-      </c>
-      <c r="C86" s="26" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="B88" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="B88" s="27" t="s">
+      <c r="C88" s="27" t="s">
         <v>162</v>
-      </c>
-      <c r="C88" s="27" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="27"/>
       <c r="B89" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C89" s="27" t="s">
         <v>164</v>
-      </c>
-      <c r="C89" s="27" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="B91" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C91" s="28" t="s">
         <v>166</v>
-      </c>
-      <c r="B91" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="C91" s="28" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="28"/>
       <c r="B92" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="C92" s="28" t="s">
         <v>169</v>
-      </c>
-      <c r="C92" s="28" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="28"/>
       <c r="B93" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C93" s="28" t="s">
         <v>171</v>
-      </c>
-      <c r="C93" s="28" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="28"/>
       <c r="B94" s="28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C94" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="28"/>
       <c r="B95" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C95" s="28" t="s">
         <v>174</v>
-      </c>
-      <c r="C95" s="28" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="28"/>
       <c r="B96" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C96" s="28" t="s">
         <v>177</v>
-      </c>
-      <c r="C96" s="28" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="28"/>
       <c r="B97" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C97" s="28" t="s">
         <v>179</v>
-      </c>
-      <c r="C97" s="28" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="28"/>
       <c r="B98" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="C98" s="28" t="s">
         <v>181</v>
-      </c>
-      <c r="C98" s="28" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="28"/>
       <c r="B99" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="C99" s="28" t="s">
         <v>183</v>
-      </c>
-      <c r="C99" s="28" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="28"/>
       <c r="B100" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C100" s="28" t="s">
         <v>185</v>
-      </c>
-      <c r="C100" s="28" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="28"/>
       <c r="B101" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="C101" s="28" t="s">
         <v>187</v>
-      </c>
-      <c r="C101" s="28" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="28"/>
       <c r="B102" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="C102" s="28" t="s">
         <v>189</v>
-      </c>
-      <c r="C102" s="28" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="28"/>
       <c r="B103" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C103" s="28" t="s">
         <v>191</v>
-      </c>
-      <c r="C103" s="28" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B105" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="C105" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="4"/>
       <c r="B106" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C106" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="4"/>
       <c r="B107" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C107" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="4"/>
       <c r="B108" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C108" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="4"/>
       <c r="B109" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C110" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="C110" s="4" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="4"/>
       <c r="B111" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C111" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="4"/>
       <c r="B112" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C112" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="4"/>
       <c r="B113" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C113" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="4"/>
       <c r="B114" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C114" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="27">
       <c r="A115" s="4"/>
       <c r="B115" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C115" s="30" t="s">
         <v>214</v>
-      </c>
-      <c r="C115" s="30" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C116" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="4"/>
       <c r="B117" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C117" s="4" t="s">
         <v>218</v>
-      </c>
-      <c r="C117" s="4" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B119" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="B119" s="8" t="s">
+      <c r="C119" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="C119" s="8" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="8"/>
       <c r="B120" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="8"/>
       <c r="B121" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="8"/>
       <c r="B122" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C122" s="8" t="s">
         <v>229</v>
-      </c>
-      <c r="C122" s="8" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="8"/>
       <c r="B123" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C123" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="C123" s="8" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="8"/>
       <c r="B124" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C124" s="8" t="s">
         <v>233</v>
-      </c>
-      <c r="C124" s="8" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
+        <v>234</v>
+      </c>
+      <c r="B126" t="s">
         <v>235</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" s="8" t="s">
         <v>236</v>
-      </c>
-      <c r="C126" s="8" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="40.5">
       <c r="B127" t="s">
+        <v>237</v>
+      </c>
+      <c r="C127" s="29" t="s">
         <v>238</v>
-      </c>
-      <c r="C127" s="29" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="B128" t="s">
+        <v>239</v>
+      </c>
+      <c r="C128" t="s">
         <v>240</v>
-      </c>
-      <c r="C128" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="129" spans="2:3">
       <c r="B129" t="s">
+        <v>241</v>
+      </c>
+      <c r="C129" t="s">
         <v>242</v>
-      </c>
-      <c r="C129" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="130" spans="2:3">
       <c r="B130" t="s">
+        <v>243</v>
+      </c>
+      <c r="C130" t="s">
         <v>244</v>
-      </c>
-      <c r="C130" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="131" spans="2:3">
       <c r="B131" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C131" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="132" spans="2:3">
       <c r="B132" t="s">
+        <v>246</v>
+      </c>
+      <c r="C132" t="s">
         <v>247</v>
-      </c>
-      <c r="C132" t="s">
-        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2583,7 +2581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2597,7 +2595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>